<commit_message>
Update timesheet & dossier
</commit_message>
<xml_diff>
--- a/docs/bap_timesheet.xlsx
+++ b/docs/bap_timesheet.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ilona\Code\everlini\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A452E89-443B-4018-BA6C-1DC520F38778}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9145A513-6629-42B0-BE72-244B456242F1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{81811DA5-A519-4071-A1FA-887EFEFF4DD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="107">
   <si>
     <t>Datum</t>
   </si>
@@ -277,6 +282,75 @@
   </si>
   <si>
     <t>Laatste fixes aan app</t>
+  </si>
+  <si>
+    <t>Voeg functionaliteit toe aan datum knoppen op home</t>
+  </si>
+  <si>
+    <t>Code clean up</t>
+  </si>
+  <si>
+    <t>Zoeken naar nog alternatieve APIs voor events</t>
+  </si>
+  <si>
+    <t>Toevoegen van Admin table en Admin Organisation pivot</t>
+  </si>
+  <si>
+    <t>Organisation table aanpassen</t>
+  </si>
+  <si>
+    <t>Styling van profiel aanpassen</t>
+  </si>
+  <si>
+    <t>Dashboard voorzien voor organisaties</t>
+  </si>
+  <si>
+    <t>Profile get functie aanpassen + layout</t>
+  </si>
+  <si>
+    <t>Favicon instellen</t>
+  </si>
+  <si>
+    <t>User toevoegen als admin bij aanmaken van organisatie</t>
+  </si>
+  <si>
+    <t>Display admins op organisatie pagina</t>
+  </si>
+  <si>
+    <t>Fix bug bij favorieten</t>
+  </si>
+  <si>
+    <t>Display blogposts in newsfeed op profielpagina</t>
+  </si>
+  <si>
+    <t>Interests tree voorzien</t>
+  </si>
+  <si>
+    <t>Default interests tonen op homepage</t>
+  </si>
+  <si>
+    <t>Default interests verwerken in search parameters</t>
+  </si>
+  <si>
+    <t>Kleine styling aanpassingen</t>
+  </si>
+  <si>
+    <t>Minor bugfixes</t>
+  </si>
+  <si>
+    <t>Slug voorzien bij organisatie</t>
+  </si>
+  <si>
+    <t>Interesses toevoegen aan events</t>
+  </si>
+  <si>
+    <t>Interesses toevoegen aan users</t>
+  </si>
+  <si>
+    <t>Zoeken door event interesses</t>
+  </si>
+  <si>
+    <t>Dossier aanpassen</t>
   </si>
 </sst>
 </file>
@@ -781,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0834EE37-AA56-4F44-80E5-EF5F7D5EDBDA}">
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="G121" sqref="G121"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,13 +2246,272 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="11"/>
-      <c r="B123" s="10" t="s">
+      <c r="A123" s="8">
+        <v>43315</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C123" s="4">
+        <f>0.5+0.25+0.5</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="8">
+        <v>43315</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C124" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="8">
+        <v>43316</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C125" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="8">
+        <v>43316</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C126" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="8">
+        <v>43316</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C127" s="4">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="8">
+        <v>43319</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C128" s="4">
+        <f>0.25+0.75+0.5</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="8">
+        <v>43319</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C129" s="4">
+        <f>0.25+0.75+0.5+0.25</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="8">
+        <v>43320</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C130" s="4">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="8">
+        <v>43321</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C131" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="8">
+        <v>43321</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C132" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="8">
+        <v>43321</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C133" s="4">
+        <f>1.5</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="8">
+        <v>43321</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C134" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="8">
+        <v>43321</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C135" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="8">
+        <v>43322</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C136" s="4">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="8">
+        <v>43323</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C137" s="4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="8">
+        <v>43323</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C138" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="8">
+        <v>43332</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C139" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="8">
+        <v>43332</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C140" s="4">
+        <f>0.25+0.75</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="8">
+        <v>43332</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C141" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="8">
+        <v>43332</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C142" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="8">
+        <v>43332</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C143" s="4">
+        <f>0.25+0.25+0.5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="8">
+        <v>43332</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C144" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="8">
+        <v>43332</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C145" s="4">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="11"/>
+      <c r="B146" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C123" s="5">
-        <f>SUM(C2:C122)</f>
-        <v>131.75</v>
+      <c r="C146" s="5">
+        <f>SUM(C2:C145)</f>
+        <v>154.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>